<commit_message>
quick check with ballpark numbers, TNM
</commit_message>
<xml_diff>
--- a/target_netmigration/TNM_workerjobbalance.xlsx
+++ b/target_netmigration/TNM_workerjobbalance.xlsx
@@ -368,7 +368,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,7 +407,7 @@
         <v>2030</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>75000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -418,7 +418,7 @@
         <v>2035</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -429,7 +429,7 @@
         <v>2040</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -440,7 +440,7 @@
         <v>2045</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -451,7 +451,7 @@
         <v>2050</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -473,7 +473,7 @@
         <v>2030</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -484,7 +484,7 @@
         <v>2035</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -495,7 +495,7 @@
         <v>2040</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -506,7 +506,7 @@
         <v>2045</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -517,7 +517,7 @@
         <v>2050</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -539,7 +539,7 @@
         <v>2030</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -550,7 +550,7 @@
         <v>2035</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -561,7 +561,7 @@
         <v>2040</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -572,7 +572,7 @@
         <v>2045</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -583,7 +583,7 @@
         <v>2050</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -605,7 +605,7 @@
         <v>2030</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -616,7 +616,7 @@
         <v>2035</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -627,7 +627,7 @@
         <v>2040</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -638,7 +638,7 @@
         <v>2045</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -877,16 +877,16 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097B1C0-D82B-4862-B210-738A5A3A3605}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
trying another number tweak
</commit_message>
<xml_diff>
--- a/target_netmigration/TNM_workerjobbalance.xlsx
+++ b/target_netmigration/TNM_workerjobbalance.xlsx
@@ -368,7 +368,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,7 +407,7 @@
         <v>2030</v>
       </c>
       <c r="C3">
-        <v>75000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -418,7 +418,7 @@
         <v>2035</v>
       </c>
       <c r="C4">
-        <v>175000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -429,7 +429,7 @@
         <v>2040</v>
       </c>
       <c r="C5">
-        <v>250000</v>
+        <v>275000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -440,7 +440,7 @@
         <v>2045</v>
       </c>
       <c r="C6">
-        <v>250000</v>
+        <v>325000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -451,7 +451,7 @@
         <v>2050</v>
       </c>
       <c r="C7">
-        <v>250000</v>
+        <v>375000</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -473,7 +473,7 @@
         <v>2030</v>
       </c>
       <c r="C9">
-        <v>20000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -484,7 +484,7 @@
         <v>2035</v>
       </c>
       <c r="C10">
-        <v>25000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -495,7 +495,7 @@
         <v>2040</v>
       </c>
       <c r="C11">
-        <v>30000</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -517,7 +517,7 @@
         <v>2050</v>
       </c>
       <c r="C13">
-        <v>8000</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -561,7 +561,7 @@
         <v>2040</v>
       </c>
       <c r="C17">
-        <v>18000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -572,7 +572,7 @@
         <v>2045</v>
       </c>
       <c r="C18">
-        <v>21000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -583,7 +583,7 @@
         <v>2050</v>
       </c>
       <c r="C19">
-        <v>24000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -594,7 +594,7 @@
         <v>2025</v>
       </c>
       <c r="C20">
-        <v>5000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -605,7 +605,7 @@
         <v>2030</v>
       </c>
       <c r="C21">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -616,7 +616,7 @@
         <v>2035</v>
       </c>
       <c r="C22">
-        <v>12000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -627,7 +627,7 @@
         <v>2040</v>
       </c>
       <c r="C23">
-        <v>15000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -638,7 +638,7 @@
         <v>2045</v>
       </c>
       <c r="C24">
-        <v>18000</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -649,7 +649,7 @@
         <v>2050</v>
       </c>
       <c r="C25">
-        <v>20000</v>
+        <v>33000</v>
       </c>
     </row>
   </sheetData>
@@ -663,21 +663,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007E4401432919E48A67AF1BA2141DC10" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9cd1da069ec09c636c0b94a4ab15d117">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b87684af-bef0-40b7-97cd-63b35f783779" xmlns:ns4="29b2ff15-f619-4740-bc35-6887da9102a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51a9c14bdc4a76ccc9b88ddfd170d770" ns3:_="" ns4:_="">
     <xsd:import namespace="b87684af-bef0-40b7-97cd-63b35f783779"/>
@@ -874,32 +859,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0553BE-6FFF-4BB6-8FF1-82E82A73BAD5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097B1C0-D82B-4862-B210-738A5A3A3605}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEFEEEAA-8617-415F-930B-22011CE55E54}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -916,4 +891,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097B1C0-D82B-4862-B210-738A5A3A3605}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0553BE-6FFF-4BB6-8FF1-82E82A73BAD5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
re-run with workers/jobs balance
</commit_message>
<xml_diff>
--- a/target_netmigration/TNM_workerjobbalance.xlsx
+++ b/target_netmigration/TNM_workerjobbalance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24228" windowHeight="10836"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24225" windowHeight="10830"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -367,17 +367,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -388,7 +388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -396,10 +396,10 @@
         <v>2025</v>
       </c>
       <c r="C2">
-        <v>-25000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -410,7 +410,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -421,7 +421,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -432,7 +432,7 @@
         <v>275000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -440,10 +440,10 @@
         <v>2045</v>
       </c>
       <c r="C6">
-        <v>325000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -451,10 +451,10 @@
         <v>2050</v>
       </c>
       <c r="C7">
-        <v>375000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>325000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -462,10 +462,10 @@
         <v>2025</v>
       </c>
       <c r="C8">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -473,10 +473,10 @@
         <v>2030</v>
       </c>
       <c r="C9">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -484,10 +484,10 @@
         <v>2035</v>
       </c>
       <c r="C10">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -495,10 +495,10 @@
         <v>2040</v>
       </c>
       <c r="C11">
-        <v>33000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -506,10 +506,10 @@
         <v>2045</v>
       </c>
       <c r="C12">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -517,10 +517,10 @@
         <v>2050</v>
       </c>
       <c r="C13">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -531,7 +531,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -542,7 +542,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -553,7 +553,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -564,7 +564,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -575,7 +575,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -583,10 +583,10 @@
         <v>2050</v>
       </c>
       <c r="C19">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -597,7 +597,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -605,10 +605,10 @@
         <v>2030</v>
       </c>
       <c r="C21">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -616,10 +616,10 @@
         <v>2035</v>
       </c>
       <c r="C22">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -630,7 +630,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -638,10 +638,10 @@
         <v>2045</v>
       </c>
       <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -663,21 +663,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007E4401432919E48A67AF1BA2141DC10" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9cd1da069ec09c636c0b94a4ab15d117">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b87684af-bef0-40b7-97cd-63b35f783779" xmlns:ns4="29b2ff15-f619-4740-bc35-6887da9102a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51a9c14bdc4a76ccc9b88ddfd170d770" ns3:_="" ns4:_="">
     <xsd:import namespace="b87684af-bef0-40b7-97cd-63b35f783779"/>
@@ -874,32 +859,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0553BE-6FFF-4BB6-8FF1-82E82A73BAD5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097B1C0-D82B-4862-B210-738A5A3A3605}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEFEEEAA-8617-415F-930B-22011CE55E54}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -916,4 +891,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097B1C0-D82B-4862-B210-738A5A3A3605}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0553BE-6FFF-4BB6-8FF1-82E82A73BAD5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
another tweak to workerjobbalance
</commit_message>
<xml_diff>
--- a/target_netmigration/TNM_workerjobbalance.xlsx
+++ b/target_netmigration/TNM_workerjobbalance.xlsx
@@ -368,7 +368,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +594,7 @@
         <v>2025</v>
       </c>
       <c r="C20">
-        <v>10000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -605,7 +605,7 @@
         <v>2030</v>
       </c>
       <c r="C21">
-        <v>15000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
         <v>2035</v>
       </c>
       <c r="C22">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>2040</v>
       </c>
       <c r="C23">
-        <v>5000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -638,7 +638,7 @@
         <v>2045</v>
       </c>
       <c r="C24">
-        <v>5000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
         <v>2050</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
   </sheetData>
@@ -663,6 +663,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007E4401432919E48A67AF1BA2141DC10" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9cd1da069ec09c636c0b94a4ab15d117">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b87684af-bef0-40b7-97cd-63b35f783779" xmlns:ns4="29b2ff15-f619-4740-bc35-6887da9102a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51a9c14bdc4a76ccc9b88ddfd170d770" ns3:_="" ns4:_="">
     <xsd:import namespace="b87684af-bef0-40b7-97cd-63b35f783779"/>
@@ -859,22 +874,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0553BE-6FFF-4BB6-8FF1-82E82A73BAD5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097B1C0-D82B-4862-B210-738A5A3A3605}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEFEEEAA-8617-415F-930B-22011CE55E54}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -891,29 +916,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097B1C0-D82B-4862-B210-738A5A3A3605}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0553BE-6FFF-4BB6-8FF1-82E82A73BAD5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tweak to TNM values, running Balance model with different BaseMigs
</commit_message>
<xml_diff>
--- a/target_netmigration/TNM_workerjobbalance.xlsx
+++ b/target_netmigration/TNM_workerjobbalance.xlsx
@@ -368,7 +368,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,7 +451,7 @@
         <v>2050</v>
       </c>
       <c r="C7">
-        <v>375000</v>
+        <v>350000</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>2040</v>
       </c>
       <c r="C23">
-        <v>5000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -638,7 +638,7 @@
         <v>2045</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
         <v>2050</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
   </sheetData>
@@ -663,12 +663,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007E4401432919E48A67AF1BA2141DC10" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9cd1da069ec09c636c0b94a4ab15d117">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b87684af-bef0-40b7-97cd-63b35f783779" xmlns:ns4="29b2ff15-f619-4740-bc35-6887da9102a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51a9c14bdc4a76ccc9b88ddfd170d770" ns3:_="" ns4:_="">
     <xsd:import namespace="b87684af-bef0-40b7-97cd-63b35f783779"/>
@@ -865,6 +859,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -875,23 +875,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097B1C0-D82B-4862-B210-738A5A3A3605}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEFEEEAA-8617-415F-930B-22011CE55E54}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -910,6 +893,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097B1C0-D82B-4862-B210-738A5A3A3605}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0553BE-6FFF-4BB6-8FF1-82E82A73BAD5}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
re-ran projection with updated TNMs and using 3 allocation periods
</commit_message>
<xml_diff>
--- a/target_netmigration/TNM_workerjobbalance.xlsx
+++ b/target_netmigration/TNM_workerjobbalance.xlsx
@@ -368,7 +368,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +407,7 @@
         <v>2030</v>
       </c>
       <c r="C3">
-        <v>150000</v>
+        <v>115000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -418,7 +418,7 @@
         <v>2035</v>
       </c>
       <c r="C4">
-        <v>250000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -429,7 +429,7 @@
         <v>2040</v>
       </c>
       <c r="C5">
-        <v>275000</v>
+        <v>225000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -440,7 +440,7 @@
         <v>2045</v>
       </c>
       <c r="C6">
-        <v>325000</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -451,7 +451,7 @@
         <v>2050</v>
       </c>
       <c r="C7">
-        <v>350000</v>
+        <v>225000</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -462,7 +462,7 @@
         <v>2025</v>
       </c>
       <c r="C8">
-        <v>10000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -495,7 +495,7 @@
         <v>2040</v>
       </c>
       <c r="C11">
-        <v>33000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -506,7 +506,7 @@
         <v>2045</v>
       </c>
       <c r="C12">
-        <v>30000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -583,7 +583,7 @@
         <v>2050</v>
       </c>
       <c r="C19">
-        <v>10000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
         <v>2035</v>
       </c>
       <c r="C22">
-        <v>15000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>2040</v>
       </c>
       <c r="C23">
-        <v>8000</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -638,7 +638,7 @@
         <v>2045</v>
       </c>
       <c r="C24">
-        <v>6000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tweak of TNM numbers, worker job balance
</commit_message>
<xml_diff>
--- a/target_netmigration/TNM_workerjobbalance.xlsx
+++ b/target_netmigration/TNM_workerjobbalance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24225" windowHeight="10830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24228" windowHeight="10836"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,16 +368,16 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -388,7 +388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -399,7 +399,7 @@
         <v>-25000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -410,7 +410,7 @@
         <v>115000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -421,7 +421,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -432,7 +432,7 @@
         <v>225000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -443,7 +443,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -454,7 +454,7 @@
         <v>225000</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -462,10 +462,10 @@
         <v>2025</v>
       </c>
       <c r="C8">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -473,10 +473,10 @@
         <v>2030</v>
       </c>
       <c r="C9">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -484,10 +484,10 @@
         <v>2035</v>
       </c>
       <c r="C10">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -495,10 +495,10 @@
         <v>2040</v>
       </c>
       <c r="C11">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -506,10 +506,10 @@
         <v>2045</v>
       </c>
       <c r="C12">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -517,10 +517,10 @@
         <v>2050</v>
       </c>
       <c r="C13">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -531,7 +531,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -539,10 +539,10 @@
         <v>2030</v>
       </c>
       <c r="C15">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -550,10 +550,10 @@
         <v>2035</v>
       </c>
       <c r="C16">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -561,10 +561,10 @@
         <v>2040</v>
       </c>
       <c r="C17">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -575,7 +575,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -586,7 +586,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -594,10 +594,10 @@
         <v>2025</v>
       </c>
       <c r="C20">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -605,10 +605,10 @@
         <v>2030</v>
       </c>
       <c r="C21">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -616,10 +616,10 @@
         <v>2035</v>
       </c>
       <c r="C22">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -627,10 +627,10 @@
         <v>2040</v>
       </c>
       <c r="C23">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -641,7 +641,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -663,6 +663,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007E4401432919E48A67AF1BA2141DC10" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9cd1da069ec09c636c0b94a4ab15d117">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b87684af-bef0-40b7-97cd-63b35f783779" xmlns:ns4="29b2ff15-f619-4740-bc35-6887da9102a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51a9c14bdc4a76ccc9b88ddfd170d770" ns3:_="" ns4:_="">
     <xsd:import namespace="b87684af-bef0-40b7-97cd-63b35f783779"/>
@@ -859,22 +874,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0553BE-6FFF-4BB6-8FF1-82E82A73BAD5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097B1C0-D82B-4862-B210-738A5A3A3605}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEFEEEAA-8617-415F-930B-22011CE55E54}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -891,29 +916,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097B1C0-D82B-4862-B210-738A5A3A3605}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0553BE-6FFF-4BB6-8FF1-82E82A73BAD5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated 30-39 override, new TNM values
</commit_message>
<xml_diff>
--- a/target_netmigration/TNM_workerjobbalance.xlsx
+++ b/target_netmigration/TNM_workerjobbalance.xlsx
@@ -368,7 +368,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +407,7 @@
         <v>2030</v>
       </c>
       <c r="C3">
-        <v>75000</v>
+        <v>130000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -418,7 +418,7 @@
         <v>2035</v>
       </c>
       <c r="C4">
-        <v>100000</v>
+        <v>160000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -663,6 +663,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007E4401432919E48A67AF1BA2141DC10" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9cd1da069ec09c636c0b94a4ab15d117">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b87684af-bef0-40b7-97cd-63b35f783779" xmlns:ns4="29b2ff15-f619-4740-bc35-6887da9102a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="51a9c14bdc4a76ccc9b88ddfd170d770" ns3:_="" ns4:_="">
     <xsd:import namespace="b87684af-bef0-40b7-97cd-63b35f783779"/>
@@ -859,22 +874,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097B1C0-D82B-4862-B210-738A5A3A3605}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0553BE-6FFF-4BB6-8FF1-82E82A73BAD5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEFEEEAA-8617-415F-930B-22011CE55E54}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -891,29 +916,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C0553BE-6FFF-4BB6-8FF1-82E82A73BAD5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B097B1C0-D82B-4862-B210-738A5A3A3605}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="29b2ff15-f619-4740-bc35-6887da9102a1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b87684af-bef0-40b7-97cd-63b35f783779"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>